<commit_message>
added stresstest for ARE GUI start model
</commit_message>
<xml_diff>
--- a/Tests/integrationTests/02_ARE GUI/Test_cases_ARE_GUI.xlsx
+++ b/Tests/integrationTests/02_ARE GUI/Test_cases_ARE_GUI.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Number</t>
   </si>
@@ -252,6 +252,20 @@
     <t>Windows OS
 ARE start file: Are.exe (start.sh - Linux)
 demomenu.acs (Should be default autostart model)</t>
+  </si>
+  <si>
+    <t>ARE_GUI_7</t>
+  </si>
+  <si>
+    <t>Stresstest Start model</t>
+  </si>
+  <si>
+    <t>1. Execute Test ARE_GUI_2 by clicking 10 times onto 'Start' button as fast as possible</t>
+  </si>
+  <si>
+    <t>The model must be started 10 times sequentially and successfully
+The last model start must have a clean state and must not have orphaned GUI elements in the ARE GUI  panel
+The ARE must not crash</t>
   </si>
 </sst>
 </file>
@@ -619,7 +633,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -630,7 +644,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,11 +809,21 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="A13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="120.95" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Test cases for installer renamed and fixed test cases of ARE_startup
</commit_message>
<xml_diff>
--- a/Tests/integrationTests/02_ARE GUI/Test_cases_ARE_GUI.xlsx
+++ b/Tests/integrationTests/02_ARE GUI/Test_cases_ARE_GUI.xlsx
@@ -157,9 +157,6 @@
     <t>Start model</t>
   </si>
   <si>
-    <t>Pause model/Resume model</t>
-  </si>
-  <si>
     <t>ARE_GUI_2</t>
   </si>
   <si>
@@ -189,11 +186,6 @@
   <si>
     <t>1. The model must stop running
 2. CameraMouse: The LED must be off and the ARE GUI panel empty, the video frame window must be closed</t>
-  </si>
-  <si>
-    <t>1. Execute test ARE_GUI_2
-2. Right click on ARE GUI background panel
-3. Click on 'start button'</t>
   </si>
   <si>
     <t>1. The model must be started successfully.
@@ -222,17 +214,6 @@
 CameraMouse: The LED must be off and the ARE GUI panel empty, the video frame window must be closed</t>
   </si>
   <si>
-    <t>1. Execute test ARE_GUI_1
-2. Right click on ARE GUI background panel
-3. Click on 'stop button'</t>
-  </si>
-  <si>
-    <t>1. Execute test ARE_GUI_1
-2. Right click on ARE GUI background panel
-3. Click on 'resume button'
-4. Click on 'start button'</t>
-  </si>
-  <si>
     <t>ARE_GUI_6</t>
   </si>
   <si>
@@ -272,18 +253,37 @@
     <t>Environment (OS + Version, Architecture, Java Version):</t>
   </si>
   <si>
-    <t>1. Execute test ARE_GUI_1
-2. Right click on ARE GUI background panel
-3. Click on 'resume button'
-4. Click on 'stop button'</t>
-  </si>
-  <si>
     <t>ARE start file: start.bat (start.sh - Linux)</t>
   </si>
   <si>
     <t>Windows OS
 ARE start file: start.bat (start.sh - Linux)
 demomenu.acs (Should be default autostart model)</t>
+  </si>
+  <si>
+    <t>Pause model/Start model</t>
+  </si>
+  <si>
+    <t>1. Execute test ARE_GUI_1
+2. Right click on ARE GUI background panel
+3. Click on 'Pause Model' button
+4. Click on 'Start Model' button</t>
+  </si>
+  <si>
+    <t>1. Execute test ARE_GUI_2
+2. Right click on ARE GUI background panel
+3. Click on 'Start Model' button</t>
+  </si>
+  <si>
+    <t>1. Execute test ARE_GUI_1
+2. Right click on ARE GUI background panel
+3. Click on 'Pause Model' button
+4. Click on 'Stop Model' button</t>
+  </si>
+  <si>
+    <t>1. Execute test ARE_GUI_1
+2. Right click on ARE GUI background panel
+3. Click on 'Stop Model' button</t>
   </si>
 </sst>
 </file>
@@ -662,7 +662,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -673,7 +673,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,10 +690,10 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="32.25" x14ac:dyDescent="0.4">
@@ -704,7 +704,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.4">
@@ -715,7 +715,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -749,121 +749,121 @@
         <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="101.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F13" s="5"/>
     </row>

</xml_diff>